<commit_message>
mr_parser addition of tenge
</commit_message>
<xml_diff>
--- a/code/LME/parser_beta/data/cb_curr.xlsx
+++ b/code/LME/parser_beta/data/cb_curr.xlsx
@@ -586,10 +586,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="E8" t="n">
-        <v>55.006</v>
+        <v>52.5113</v>
       </c>
     </row>
     <row r="9">
@@ -738,10 +738,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="E16" t="n">
-        <v>56.2953</v>
+        <v>53.2682</v>
       </c>
     </row>
     <row r="17">
@@ -890,10 +890,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="E24" t="n">
-        <v>56.9219</v>
+        <v>53.7028</v>
       </c>
     </row>
     <row r="25">
@@ -1042,10 +1042,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="E32" t="n">
-        <v>55.6248</v>
+        <v>53.0609</v>
       </c>
     </row>
     <row r="33">

</xml_diff>